<commit_message>
update entidade excel e compra sql
</commit_message>
<xml_diff>
--- a/Requisitos/Entidades.xlsx
+++ b/Requisitos/Entidades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicia\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicia\OneDrive\Área de Trabalho\Rifa-Manager-main\Rifa-Manager\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4E0305-7E59-4064-855C-BE5D4BB6DCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58D37A1-1CCA-4C4A-A138-F9BDE5560F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B048BBEE-A412-47BC-B1E5-CE6A073615E9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="78">
   <si>
     <t>Tabela</t>
   </si>
@@ -247,6 +247,27 @@
   </si>
   <si>
     <t xml:space="preserve">identificação do usuário que comprou o bilhete </t>
+  </si>
+  <si>
+    <t>Compra</t>
+  </si>
+  <si>
+    <t>Informação de uma Compra realizada por um Cliente</t>
+  </si>
+  <si>
+    <t>id_compra</t>
+  </si>
+  <si>
+    <t>Status da compra</t>
+  </si>
+  <si>
+    <t>identificação do cliente que fez a compra</t>
+  </si>
+  <si>
+    <t>identificação da rifa da compra</t>
+  </si>
+  <si>
+    <t>identificação da compra</t>
   </si>
 </sst>
 </file>
@@ -906,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD238F1-374A-4F00-B265-9AC1B38F165A}">
   <dimension ref="B1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -918,7 +939,7 @@
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="28.109375" customWidth="1"/>
     <col min="8" max="8" width="18.109375" customWidth="1"/>
-    <col min="9" max="9" width="36.109375" customWidth="1"/>
+    <col min="9" max="9" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5546875" customWidth="1"/>
     <col min="11" max="11" width="19.109375" customWidth="1"/>
     <col min="12" max="12" width="23.33203125" customWidth="1"/>
@@ -1353,6 +1374,15 @@
       <c r="D26" s="24"/>
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
+      <c r="H26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="25"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
@@ -1364,6 +1394,15 @@
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="27"/>
+      <c r="H27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="27"/>
     </row>
     <row r="28" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
@@ -1373,6 +1412,13 @@
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="29"/>
+      <c r="H28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29"/>
     </row>
     <row r="29" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="30" t="s">
@@ -1382,6 +1428,13 @@
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
       <c r="F29" s="32"/>
+      <c r="H29" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="32"/>
     </row>
     <row r="30" spans="2:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="9" t="s">
@@ -1399,6 +1452,21 @@
       <c r="F30" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="H30" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
@@ -1414,6 +1482,19 @@
       <c r="F31" s="14" t="s">
         <v>67</v>
       </c>
+      <c r="H31" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="32" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
@@ -1429,8 +1510,21 @@
       <c r="F32" s="16" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H32" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="L32" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
         <v>69</v>
       </c>
@@ -1442,8 +1536,19 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="16"/>
-    </row>
-    <row r="34" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H33" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="L33" s="16"/>
+    </row>
+    <row r="34" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
         <v>11</v>
       </c>
@@ -1457,8 +1562,21 @@
       <c r="F34" s="16" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H34" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K34" s="1"/>
+      <c r="L34" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="s">
         <v>29</v>
       </c>
@@ -1472,8 +1590,21 @@
       <c r="F35" s="16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H35" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="15" t="s">
         <v>18</v>
       </c>
@@ -1487,8 +1618,21 @@
       <c r="F36" s="16" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H36" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="17" t="s">
         <v>19</v>
       </c>
@@ -1502,34 +1646,51 @@
       <c r="F37" s="19" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="H37" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="J37" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K37" s="18"/>
+      <c r="L37" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="8"/>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="8"/>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="B5:F5"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="B11:F11"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
docs new documentos requisitos
</commit_message>
<xml_diff>
--- a/Requisitos/Entidades.xlsx
+++ b/Requisitos/Entidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicia\OneDrive\Área de Trabalho\Rifa-Manager-main\Rifa-Manager\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3542233A-A146-4E35-A6CD-443C33790697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BA022C-0B1F-4980-92DD-24EF9F99DD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B048BBEE-A412-47BC-B1E5-CE6A073615E9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="76">
   <si>
     <t>Tabela</t>
   </si>
@@ -72,9 +72,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>cpf</t>
-  </si>
-  <si>
     <t>reset_token</t>
   </si>
   <si>
@@ -105,18 +102,9 @@
     <t>rifa_id</t>
   </si>
   <si>
-    <t>numberOfTicket</t>
-  </si>
-  <si>
     <t>expire</t>
   </si>
   <si>
-    <t>id_bilhete</t>
-  </si>
-  <si>
-    <t>id_rifa</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -219,30 +207,18 @@
     <t>not null / unique</t>
   </si>
   <si>
-    <t>id_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">identificação do usuário que comprou o bilhete </t>
-  </si>
-  <si>
     <t>Compra</t>
   </si>
   <si>
     <t>Informação de uma Compra realizada por um Cliente</t>
   </si>
   <si>
-    <t>id_compra</t>
-  </si>
-  <si>
     <t>Status da compra</t>
   </si>
   <si>
     <t>identificação do cliente que fez a compra</t>
   </si>
   <si>
-    <t>identificação da rifa da compra</t>
-  </si>
-  <si>
     <t>identificação da compra</t>
   </si>
   <si>
@@ -270,7 +246,22 @@
     <t>cpf do cliente</t>
   </si>
   <si>
-    <t>se o cliente é admin ou não</t>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>numerobilhetes</t>
+  </si>
+  <si>
+    <t>compra_id</t>
+  </si>
+  <si>
+    <t>bilhete_id</t>
+  </si>
+  <si>
+    <t>CPF</t>
   </si>
 </sst>
 </file>
@@ -587,6 +578,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,18 +603,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -930,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD238F1-374A-4F00-B265-9AC1B38F165A}">
   <dimension ref="B1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -953,37 +944,37 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="30"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="28"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" spans="2:12" ht="52.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
@@ -1007,73 +998,73 @@
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+      <c r="C8" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
       <c r="H8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="30"/>
+      <c r="I8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
+      <c r="C9" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="27"/>
       <c r="H9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="32"/>
+      <c r="I9" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
       <c r="H10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="25"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="H11" s="26" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="H11" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="28"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" spans="2:12" ht="55.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="9" t="s">
@@ -1089,7 +1080,7 @@
         <v>5</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>3</v>
@@ -1104,35 +1095,35 @@
         <v>5</v>
       </c>
       <c r="L12" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
@@ -1140,27 +1131,27 @@
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H14" s="15" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="16" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
@@ -1168,29 +1159,29 @@
         <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E15" s="1">
         <v>20</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H15" s="15" t="s">
         <v>9</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:12" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1198,172 +1189,175 @@
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="16" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1">
         <v>11</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K17" s="1"/>
       <c r="L17" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="16"/>
       <c r="H18" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="16"/>
       <c r="H19" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E23" s="18">
         <v>11</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="I23" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1371,73 +1365,73 @@
       <c r="B26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
+      <c r="C26" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25"/>
       <c r="H26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="30"/>
+      <c r="I26" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="25"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
+      <c r="C27" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="27"/>
       <c r="H27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I27" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="32"/>
+      <c r="I27" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="27"/>
     </row>
     <row r="28" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="25"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
       <c r="H28" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="25"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="29"/>
     </row>
     <row r="29" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="28"/>
-      <c r="H29" s="26" t="s">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
+      <c r="H29" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="28"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="32"/>
     </row>
     <row r="30" spans="2:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="9" t="s">
@@ -1473,196 +1467,170 @@
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="12" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K31" s="13"/>
       <c r="L31" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I32" s="21" t="s">
-        <v>68</v>
+        <v>34</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" s="21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B33" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="16"/>
-      <c r="H33" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="J33" s="1" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12" ht="28.8" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B36" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="15" t="s">
+      <c r="C36" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H36" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K36" s="1"/>
-      <c r="L36" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" s="18"/>
-      <c r="F37" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="J37" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" s="18"/>
-      <c r="L37" s="19" t="s">
-        <v>39</v>
+      <c r="I36" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="K36" s="18"/>
+      <c r="L36" s="19" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.3">
@@ -1676,16 +1644,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="I10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="C10:F10"/>
@@ -1696,6 +1654,16 @@
     <mergeCell ref="H29:L29"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="I9:L9"/>
+    <mergeCell ref="I10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="B5:F5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>